<commit_message>
normalization solved and hk_Enzy new
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G_0.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G_0.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -69,7 +75,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">

</xml_diff>